<commit_message>
live update code run
</commit_message>
<xml_diff>
--- a/stock_predictor_ai/data/cleaned/ANET.xlsx
+++ b/stock_predictor_ai/data/cleaned/ANET.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2777"/>
+  <dimension ref="A1:F2778"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55989,6 +55989,26 @@
         <v>1212153</v>
       </c>
     </row>
+    <row r="2778">
+      <c r="A2778" s="2" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B2778" t="n">
+        <v>105.6399993896484</v>
+      </c>
+      <c r="C2778" t="n">
+        <v>105.870002746582</v>
+      </c>
+      <c r="D2778" t="n">
+        <v>103.6999969482422</v>
+      </c>
+      <c r="E2778" t="n">
+        <v>103.8499984741211</v>
+      </c>
+      <c r="F2778" t="n">
+        <v>1176266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added data to placeholder data folders
</commit_message>
<xml_diff>
--- a/stock_predictor_ai/data/cleaned/ANET.xlsx
+++ b/stock_predictor_ai/data/cleaned/ANET.xlsx
@@ -63,7 +63,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2781"/>
+  <dimension ref="A1:F2776"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55969,106 +55971,6 @@
         <v>11787200</v>
       </c>
     </row>
-    <row r="2777">
-      <c r="A2777" s="2" t="n">
-        <v>45841</v>
-      </c>
-      <c r="B2777" t="n">
-        <v>102.7676010131836</v>
-      </c>
-      <c r="C2777" t="n">
-        <v>103.4899978637695</v>
-      </c>
-      <c r="D2777" t="n">
-        <v>101.3000030517578</v>
-      </c>
-      <c r="E2777" t="n">
-        <v>101.3300018310547</v>
-      </c>
-      <c r="F2777" t="n">
-        <v>1212153</v>
-      </c>
-    </row>
-    <row r="2778">
-      <c r="A2778" s="2" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B2778" t="n">
-        <v>105.6399993896484</v>
-      </c>
-      <c r="C2778" t="n">
-        <v>105.870002746582</v>
-      </c>
-      <c r="D2778" t="n">
-        <v>103.6999969482422</v>
-      </c>
-      <c r="E2778" t="n">
-        <v>103.8499984741211</v>
-      </c>
-      <c r="F2778" t="n">
-        <v>1176266</v>
-      </c>
-    </row>
-    <row r="2779">
-      <c r="A2779" s="2" t="n">
-        <v>45853</v>
-      </c>
-      <c r="B2779" t="n">
-        <v>107.370002746582</v>
-      </c>
-      <c r="C2779" t="n">
-        <v>109.1999969482422</v>
-      </c>
-      <c r="D2779" t="n">
-        <v>106.3499984741211</v>
-      </c>
-      <c r="E2779" t="n">
-        <v>108.5</v>
-      </c>
-      <c r="F2779" t="n">
-        <v>7450900</v>
-      </c>
-    </row>
-    <row r="2780">
-      <c r="A2780" s="2" t="n">
-        <v>45859</v>
-      </c>
-      <c r="B2780" t="n">
-        <v>112.0599975585938</v>
-      </c>
-      <c r="C2780" t="n">
-        <v>112.6999969482422</v>
-      </c>
-      <c r="D2780" t="n">
-        <v>110.6400985717773</v>
-      </c>
-      <c r="E2780" t="n">
-        <v>111.75</v>
-      </c>
-      <c r="F2780" t="n">
-        <v>1698628</v>
-      </c>
-    </row>
-    <row r="2781">
-      <c r="A2781" s="2" t="n">
-        <v>45902</v>
-      </c>
-      <c r="B2781" t="n">
-        <v>136.1300048828125</v>
-      </c>
-      <c r="C2781" t="n">
-        <v>136.1999969482422</v>
-      </c>
-      <c r="D2781" t="n">
-        <v>131</v>
-      </c>
-      <c r="E2781" t="n">
-        <v>132.4100036621094</v>
-      </c>
-      <c r="F2781" t="n">
-        <v>4013146</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>